<commit_message>
chore: update marketing controller and excel data files
</commit_message>
<xml_diff>
--- a/Data_Meta/Dream-uilt-2022-Campañas-1-ene-2025---8-ene-2026.xlsx
+++ b/Data_Meta/Dream-uilt-2022-Campañas-1-ene-2025---8-ene-2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F429162-10BD-41CF-937C-A117BEB23DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F43325-1FF7-470D-B99B-38ED029959A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A35" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>